<commit_message>
Modified scheme add code and extent reports code added
</commit_message>
<xml_diff>
--- a/DataSheet/datasheet.xlsx
+++ b/DataSheet/datasheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhulappa R N\Project2\demotest\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2A7CDDE-988C-400D-BB0E-81E409968068}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B56CBE-8E5F-4507-BFBE-BFDF9AD113AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{69EE3CF9-0DF2-4D5E-9514-942DD0DF7A95}"/>
   </bookViews>
@@ -80,9 +80,6 @@
     <t>End Month</t>
   </si>
   <si>
-    <t>ProductAuto2</t>
-  </si>
-  <si>
     <t>SchemeAutomation123</t>
   </si>
   <si>
@@ -99,6 +96,9 @@
   </si>
   <si>
     <t>"29"</t>
+  </si>
+  <si>
+    <t>product2</t>
   </si>
 </sst>
 </file>
@@ -539,7 +539,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -577,18 +577,18 @@
         <v>16</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -603,16 +603,16 @@
         <v>14</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
         <v>21</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated fes test cases
</commit_message>
<xml_diff>
--- a/DataSheet/datasheet.xlsx
+++ b/DataSheet/datasheet.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dhulappa R N\Project2\demotest\DataSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5B56CBE-8E5F-4507-BFBE-BFDF9AD113AD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD08A466-5D04-42CE-88DD-6AD3161CCABA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{69EE3CF9-0DF2-4D5E-9514-942DD0DF7A95}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{69EE3CF9-0DF2-4D5E-9514-942DD0DF7A95}"/>
   </bookViews>
   <sheets>
     <sheet name="login" sheetId="1" r:id="rId1"/>
     <sheet name="Browser" sheetId="2" r:id="rId2"/>
     <sheet name="CreateScheme" sheetId="3" r:id="rId3"/>
+    <sheet name="AssignScheme" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,14 +28,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>username</t>
   </si>
   <si>
-    <t>pumaadmin</t>
-  </si>
-  <si>
     <t>mobisy</t>
   </si>
   <si>
@@ -99,6 +97,42 @@
   </si>
   <si>
     <t>product2</t>
+  </si>
+  <si>
+    <t>warehouse / distributor</t>
+  </si>
+  <si>
+    <t>ZoneName</t>
+  </si>
+  <si>
+    <t>northzone</t>
+  </si>
+  <si>
+    <t>SubZone Name</t>
+  </si>
+  <si>
+    <t>subzone1</t>
+  </si>
+  <si>
+    <t>Holder Name</t>
+  </si>
+  <si>
+    <t>HolderType</t>
+  </si>
+  <si>
+    <t>warehouse1</t>
+  </si>
+  <si>
+    <t>Scheme Name</t>
+  </si>
+  <si>
+    <t>Scheme ID</t>
+  </si>
+  <si>
+    <t>"5"</t>
+  </si>
+  <si>
+    <t>myclientadmin</t>
   </si>
 </sst>
 </file>
@@ -462,13 +496,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2D53945-3A12-4F77-A1DF-3D5595B800D4}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
@@ -476,23 +510,23 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -515,17 +549,17 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +572,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{067285A1-57A6-45EA-B69D-99FEAA7AADAD}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
@@ -553,69 +587,129 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
       <c r="G1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>16</v>
-      </c>
       <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>21</v>
-      </c>
-      <c r="J2" t="s">
-        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72FF3394-CAD9-4DBD-B6B7-373D365D1D01}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>